<commit_message>
updating DOE to reflect that building eff now has 2 files
</commit_message>
<xml_diff>
--- a/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
+++ b/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFEWS\RDM\IDB_RDM_Colombia\relationships\gcam\config\output\doe\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9576D83-D1C5-44E9-93EE-AF2740A801A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D6B142E-5E8F-2446-85F5-F828CF9E4562}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy &amp; Uncertainty" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -162,14 +156,6 @@
 Strategy_1_Low_Nuclear</t>
   </si>
   <si>
-    <t>Colombia_Bldg_ShellApplianceEff_High
-Colombia_IndustrialEff_High</t>
-  </si>
-  <si>
-    <t>Strategy_2_High_BldEE
-Strategy_2_High_IndEE</t>
-  </si>
-  <si>
     <t>Colombia_Bldg_ShellApplianceEff_Low
 Colombia_IndustrialEff_Low</t>
   </si>
@@ -285,12 +271,22 @@
   </si>
   <si>
     <t>Uncertainty_6_High_HOV-CL</t>
+  </si>
+  <si>
+    <t>Strategy_2_High_BldShellEE
+Strategy_2_High_BldApplEE
+Strategy_2_High_IndEE</t>
+  </si>
+  <si>
+    <t>Colombia_Bldg_ShellApplianceEff_High
+Bldg_Appliance_Eff_High
+Colombia_IndustrialEff_High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -389,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -431,10 +427,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{C48A9498-10D3-411B-911C-0AE0E83F320B}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -747,18 +746,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26924F1A-A824-4F48-8224-282370888CED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -814,24 +813,24 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="31.5">
+    <row r="5" spans="2:8" ht="47.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -842,13 +841,13 @@
         <v>20</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="G6" s="10"/>
     </row>
@@ -860,16 +859,16 @@
         <v>21</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -880,14 +879,14 @@
         <v>22</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -898,10 +897,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
@@ -950,16 +949,16 @@
         <v>11</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="47.25">
@@ -970,16 +969,16 @@
         <v>12</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="31.5">
@@ -993,7 +992,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="10"/>
@@ -1007,16 +1006,16 @@
         <v>14</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="47.25">
@@ -1027,16 +1026,16 @@
         <v>15</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -1047,10 +1046,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
@@ -1066,6 +1065,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4312479EF03E04E9C80EFDBABE84330" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a063b846935b1c24e04084d225ec4fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a7773017-533a-4fac-8654-0c9df14258d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ac990fe54ee2dfc432706ff1408291d" ns3:_="">
     <xsd:import namespace="a7773017-533a-4fac-8654-0c9df14258d0"/>
@@ -1243,35 +1257,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1293,9 +1282,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Clean up the building shell and appliance efficiency names to be corresponding to the summary file
</commit_message>
<xml_diff>
--- a/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
+++ b/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NEXO-UA\Github\IDB_RDM_Colombia\relationships\gcam\config\output\doe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD39A61C-AD8C-41C1-BFE6-787BAB624287}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy &amp; Uncertainty" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -278,7 +284,7 @@
 Strategy_2_High_IndEE</t>
   </si>
   <si>
-    <t>Colombia_Bldg_ShellApplianceEff_High
+    <t>Bldg_ShellEff_High
 Bldg_Appliance_Eff_High
 Colombia_IndustrialEff_High</t>
   </si>
@@ -286,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -433,7 +439,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -746,18 +752,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1065,21 +1071,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4312479EF03E04E9C80EFDBABE84330" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a063b846935b1c24e04084d225ec4fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a7773017-533a-4fac-8654-0c9df14258d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ac990fe54ee2dfc432706ff1408291d" ns3:_="">
     <xsd:import namespace="a7773017-533a-4fac-8654-0c9df14258d0"/>
@@ -1257,10 +1248,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1282,19 +1298,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update the config generator script and xlsx spreadsheet with up to date names of factors
</commit_message>
<xml_diff>
--- a/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
+++ b/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFEWS\RDM\IDB_RDM_Colombia\relationships\gcam\config\output\doe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A389F17-1D70-4840-9DA7-21690DD1993B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30164C01-A9B1-4AA4-8C10-ED99E4A291E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>Strategy_1</t>
   </si>
@@ -223,14 +223,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-transportation_UCD_CORE_ModEVcost_Colombia_noPubTrninterp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty_2_Low_EVCost
-</t>
-  </si>
-  <si>
     <t>Uncertainty_3_High_RECostSolar Uncertainty_3_High_RECostWind</t>
   </si>
   <si>
@@ -269,9 +261,6 @@
     <t>Global_ag_trade_HOV_CL_25</t>
   </si>
   <si>
-    <t>Uncertainty_6_High_HOV-CL</t>
-  </si>
-  <si>
     <t>Strategy_2_High_BldShellEE
 Strategy_2_High_BldApplEE
 Strategy_2_High_IndEE</t>
@@ -283,6 +272,9 @@
   </si>
   <si>
     <t>land_constraint_Colombia_constant</t>
+  </si>
+  <si>
+    <t>Uncertainty_6_High_HOV_sw_high_CL</t>
   </si>
 </sst>
 </file>
@@ -762,7 +754,7 @@
   <dimension ref="B3:H20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -826,10 +818,10 @@
         <v>19</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="8" t="s">
@@ -886,7 +878,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>45</v>
@@ -977,12 +969,8 @@
       <c r="E14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:8" ht="31.5">
       <c r="B15" s="12" t="s">
@@ -995,7 +983,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="10"/>
@@ -1009,16 +997,16 @@
         <v>14</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="47.25">
@@ -1029,16 +1017,16 @@
         <v>15</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="2:7">
@@ -1049,10 +1037,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>

</xml_diff>

<commit_message>
update RDM XL spreadsheet
</commit_message>
<xml_diff>
--- a/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
+++ b/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFEWS\RDM\IDB_RDM_Colombia\relationships\gcam\config\output\doe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarl762\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30164C01-A9B1-4AA4-8C10-ED99E4A291E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D5F5DB-D313-4FFE-8AA0-6FC9E05B9286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy &amp; Uncertainty" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Strategy_1</t>
   </si>
@@ -274,7 +274,19 @@
     <t>land_constraint_Colombia_constant</t>
   </si>
   <si>
-    <t>Uncertainty_6_High_HOV_sw_high_CL</t>
+    <t>Uncertainty_7_High_BioCeiling; Uncertainty 7_High_BioCeiling_link</t>
+  </si>
+  <si>
+    <t>Uncertainty_7_Low_BioCeiling; Uncertainty 7_Low_BioCeiling_link</t>
+  </si>
+  <si>
+    <t>Uncertainty_6_High_sw_high_CL</t>
+  </si>
+  <si>
+    <t>Uncertainty 7</t>
+  </si>
+  <si>
+    <t>Bio Constraint</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -374,12 +386,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -425,6 +448,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -753,20 +785,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.125" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.84765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.09765625" customWidth="1"/>
     <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="39.125" customWidth="1"/>
+    <col min="6" max="6" width="39.09765625" customWidth="1"/>
     <col min="7" max="7" width="30.25" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -789,7 +821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="31.5">
+    <row r="4" spans="2:8" ht="31.2">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -810,7 +842,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="47.25">
+    <row r="5" spans="2:8" ht="46.8">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -936,7 +968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="31.5">
+    <row r="13" spans="2:8" ht="31.2">
       <c r="B13" s="12" t="s">
         <v>6</v>
       </c>
@@ -956,7 +988,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="47.25">
+    <row r="14" spans="2:8" ht="46.8">
       <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
@@ -972,7 +1004,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="2:8" ht="31.5">
+    <row r="15" spans="2:8" ht="31.2">
       <c r="B15" s="12" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +1041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="47.25">
+    <row r="17" spans="2:7" ht="46.8">
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1040,10 +1072,24 @@
         <v>63</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="2:7" ht="36" customHeight="1">
+      <c r="B19" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
       <c r="C20" s="1"/>
@@ -1065,12 +1111,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4312479EF03E04E9C80EFDBABE84330" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a063b846935b1c24e04084d225ec4fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a7773017-533a-4fac-8654-0c9df14258d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ac990fe54ee2dfc432706ff1408291d" ns3:_="">
     <xsd:import namespace="a7773017-533a-4fac-8654-0c9df14258d0"/>
@@ -1248,6 +1288,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
   <ds:schemaRefs>
@@ -1257,22 +1303,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1288,4 +1318,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
merging summary xlsx sheet
</commit_message>
<xml_diff>
--- a/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
+++ b/relationships/gcam/config/output/doe/RDM_strategy_uncertainty_xml_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFEWS\RDM\IDB_RDM_Colombia\relationships\gcam\config\output\doe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarl762\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30164C01-A9B1-4AA4-8C10-ED99E4A291E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D5F5DB-D313-4FFE-8AA0-6FC9E05B9286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy &amp; Uncertainty" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Strategy_1</t>
   </si>
@@ -274,7 +274,19 @@
     <t>land_constraint_Colombia_constant</t>
   </si>
   <si>
-    <t>Uncertainty_6_High_HOV_sw_high_CL</t>
+    <t>Uncertainty_7_High_BioCeiling; Uncertainty 7_High_BioCeiling_link</t>
+  </si>
+  <si>
+    <t>Uncertainty_7_Low_BioCeiling; Uncertainty 7_Low_BioCeiling_link</t>
+  </si>
+  <si>
+    <t>Uncertainty_6_High_sw_high_CL</t>
+  </si>
+  <si>
+    <t>Uncertainty 7</t>
+  </si>
+  <si>
+    <t>Bio Constraint</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -374,12 +386,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -425,6 +448,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -753,20 +785,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.125" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.84765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.09765625" customWidth="1"/>
     <col min="5" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="39.125" customWidth="1"/>
+    <col min="6" max="6" width="39.09765625" customWidth="1"/>
     <col min="7" max="7" width="30.25" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -789,7 +821,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="31.5">
+    <row r="4" spans="2:8" ht="31.2">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -810,7 +842,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="47.25">
+    <row r="5" spans="2:8" ht="46.8">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -936,7 +968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="31.5">
+    <row r="13" spans="2:8" ht="31.2">
       <c r="B13" s="12" t="s">
         <v>6</v>
       </c>
@@ -956,7 +988,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="47.25">
+    <row r="14" spans="2:8" ht="46.8">
       <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
@@ -972,7 +1004,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="2:8" ht="31.5">
+    <row r="15" spans="2:8" ht="31.2">
       <c r="B15" s="12" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +1041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="47.25">
+    <row r="17" spans="2:7" ht="46.8">
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
@@ -1040,10 +1072,24 @@
         <v>63</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="2:7" ht="36" customHeight="1">
+      <c r="B19" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="2:7">
       <c r="C20" s="1"/>
@@ -1065,12 +1111,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A4312479EF03E04E9C80EFDBABE84330" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6a063b846935b1c24e04084d225ec4fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a7773017-533a-4fac-8654-0c9df14258d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ac990fe54ee2dfc432706ff1408291d" ns3:_="">
     <xsd:import namespace="a7773017-533a-4fac-8654-0c9df14258d0"/>
@@ -1248,6 +1288,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08564DE-8754-496E-B25E-7C4C54B72013}">
   <ds:schemaRefs>
@@ -1257,22 +1303,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C53095-6DBC-4A4F-8FE7-1E052F02F02E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1288,4 +1318,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABC5E852-43CE-4395-AE2E-08BA3FC088F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a7773017-533a-4fac-8654-0c9df14258d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>